<commit_message>
role change Signed-off-by: shanonder <shanonder@163.com>
</commit_message>
<xml_diff>
--- a/role.xlsx
+++ b/role.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,13 +82,16 @@
   <si>
     <t>role_source_4</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,16 +443,16 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="37.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,9 +466,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -477,7 +480,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -491,7 +494,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -505,7 +508,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -519,7 +522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>2</v>
       </c>
@@ -533,7 +536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>3</v>
       </c>
@@ -547,7 +550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>4</v>
       </c>

</xml_diff>